<commit_message>
Adding the usersData xlsx file
</commit_message>
<xml_diff>
--- a/Login Application/cmake-build-debug/output/usersData.xlsx
+++ b/Login Application/cmake-build-debug/output/usersData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Faculty-Content\2nd Semester\Structured Programming 1\Assighnments\Assignment 4\Programming_Assignment_4\Login Application\cmake-build-debug\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA3104B-4DB1-4BB7-A3AA-21137A04B871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF10B04E-9DD6-4972-B96A-4899E3FF77B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="3540" windowWidth="17280" windowHeight="9420" xr2:uid="{FF49B81A-127A-B44C-A44B-FF0F3EF8FCF9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{FF49B81A-127A-B44C-A44B-FF0F3EF8FCF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,22 +33,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Login Application Project.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>01120664373</t>
+  </si>
+  <si>
+    <t>mohamed.h.eladwy</t>
+  </si>
+  <si>
+    <t>Mohamed Eladwy</t>
+  </si>
+  <si>
+    <t>Full Name:</t>
+  </si>
+  <si>
+    <t>Phone Number:</t>
+  </si>
+  <si>
+    <t>Email:</t>
+  </si>
+  <si>
+    <t>Password:</t>
+  </si>
+  <si>
+    <t>ID:</t>
+  </si>
+  <si>
+    <t>mohamed.h.eladwy@gmail.com</t>
+  </si>
+  <si>
+    <t>Yusuf.Bdr132</t>
+  </si>
+  <si>
+    <t>Yusuf Elsayad Bdr</t>
+  </si>
+  <si>
+    <t>01142340941</t>
+  </si>
+  <si>
+    <t>yusuf.bdr.123@gmail.com</t>
+  </si>
+  <si>
+    <t>Amr.Elsayed.Elhenawy</t>
+  </si>
+  <si>
+    <t>Amr Elsayed Elhenawy</t>
+  </si>
+  <si>
+    <t>01121753452</t>
+  </si>
+  <si>
+    <t>amr.elhenawy@gmail.com</t>
+  </si>
+  <si>
+    <t>56/89/2003#Amr</t>
+  </si>
+  <si>
+    <t>15/7/2006#Yusuf</t>
+  </si>
+  <si>
+    <t>132@Hussein</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -71,13 +133,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -390,27 +457,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049FB1B4-2A61-4643-8816-8B76EC36FD4B}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="22.59765625" customWidth="1"/>
+    <col min="1" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="23" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="5" max="5" width="30" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{1875B68A-1EDC-4C43-8C75-B612DDA6FE3D}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{4F789BA7-2657-487A-9F94-359B33465E28}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{3A77A5A7-52EA-4797-BE69-CFEB2D8197B5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mohamed Hussein Ended Everything except Forget Password Function
</commit_message>
<xml_diff>
--- a/Login Application/cmake-build-debug/output/usersData.xlsx
+++ b/Login Application/cmake-build-debug/output/usersData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Faculty-Content\2nd Semester\Structured Programming 1\Assighnments\Assignment 4\Programming_Assignment_4\Login Application\cmake-build-debug\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF656DD4-BBC4-4D69-852F-361BD33E48E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECEFB48-40A5-42C1-85CE-326C46B2B650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{FF49B81A-127A-B44C-A44B-FF0F3EF8FCF9}"/>
   </bookViews>
@@ -74,34 +74,52 @@
     <t>yusuf.bdr.123@gmail.com</t>
   </si>
   <si>
-    <t>Amr.Elsayed.Elhenawy</t>
-  </si>
-  <si>
-    <t>Amr Elsayed Elhenawy</t>
-  </si>
-  <si>
-    <t>01121753452</t>
+    <t>15/7/2006#Yusuf</t>
+  </si>
+  <si>
+    <t>nlsznvwSfhhvrm123@</t>
+  </si>
+  <si>
+    <t>ahmed.nasr</t>
+  </si>
+  <si>
+    <t>Ahmad Nasr</t>
+  </si>
+  <si>
+    <t>01125697852</t>
+  </si>
+  <si>
+    <t>ahmed.nasr@gmail.com</t>
+  </si>
+  <si>
+    <t>ZsnvwMzhi123#</t>
+  </si>
+  <si>
+    <t>Blocked Mood:</t>
+  </si>
+  <si>
+    <t>amr.elhenawy</t>
+  </si>
+  <si>
+    <t>Amr Elhenawy</t>
+  </si>
+  <si>
+    <t>01234567890</t>
   </si>
   <si>
     <t>amr.elhenawy@gmail.com</t>
   </si>
   <si>
-    <t>56/89/2003#Amr</t>
-  </si>
-  <si>
-    <t>15/7/2006#Yusuf</t>
-  </si>
-  <si>
-    <t>132@Hussein</t>
-  </si>
-  <si>
-    <t>Blocked Mode:</t>
-  </si>
-  <si>
-    <t>nlsznvwSfhhvrm123+</t>
-  </si>
-  <si>
-    <t>nlsznvwSfhhvrm123@</t>
+    <t>ZniVosvmzdb123#</t>
+  </si>
+  <si>
+    <t>01234567891</t>
+  </si>
+  <si>
+    <t>amr.elhenawy123@gmail.com</t>
+  </si>
+  <si>
+    <t>zni.vosvmzdb123@tnzro.xln</t>
   </si>
 </sst>
 </file>
@@ -498,8 +516,8 @@
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="b">
-        <v>1</v>
+      <c r="F1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -516,7 +534,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -536,7 +554,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -544,21 +562,41 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mohamed Hussein Changes bdr Function
</commit_message>
<xml_diff>
--- a/Login Application/cmake-build-debug/output/usersData.xlsx
+++ b/Login Application/cmake-build-debug/output/usersData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Faculty-Content\2nd Semester\Structured Programming 1\Assighnments\Assignment 4\Programming_Assignment_4\Login Application\cmake-build-debug\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECEFB48-40A5-42C1-85CE-326C46B2B650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DBD023-902C-4CDE-B693-B4291B5511A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{FF49B81A-127A-B44C-A44B-FF0F3EF8FCF9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>01120664373</t>
   </si>
@@ -102,15 +102,6 @@
   </si>
   <si>
     <t>Amr Elhenawy</t>
-  </si>
-  <si>
-    <t>01234567890</t>
-  </si>
-  <si>
-    <t>amr.elhenawy@gmail.com</t>
-  </si>
-  <si>
-    <t>ZniVosvmzdb123#</t>
   </si>
   <si>
     <t>01234567891</t>
@@ -484,16 +475,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049FB1B4-2A61-4643-8816-8B76EC36FD4B}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="1" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="23" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
     <col min="5" max="5" width="30" style="1" customWidth="1"/>
@@ -537,7 +527,7 @@
         <v>14</v>
       </c>
       <c r="F2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -580,7 +570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -588,13 +578,13 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Adding the UsersData.xlsx File
</commit_message>
<xml_diff>
--- a/Login Application/cmake-build-debug/output/usersData.xlsx
+++ b/Login Application/cmake-build-debug/output/usersData.xlsx
@@ -111,6 +111,48 @@
   </si>
   <si>
     <t>zni.vosvmzdb123@tnzro.xln</t>
+  </si>
+  <si>
+    <t>mohamed.hussein.eladwy</t>
+  </si>
+  <si>
+    <t>01123456789</t>
+  </si>
+  <si>
+    <t>mh8579007@gmail.com</t>
+  </si>
+  <si>
+    <t>Nlsznvw123*+</t>
+  </si>
+  <si>
+    <t>mohamed.eladwy</t>
+  </si>
+  <si>
+    <t>01233456789</t>
+  </si>
+  <si>
+    <t>mohamedeljoker309@gmail.com</t>
+  </si>
+  <si>
+    <t>Nlsznvw123#</t>
+  </si>
+  <si>
+    <t>yusuf.bdr</t>
+  </si>
+  <si>
+    <t>Yusuf Badr</t>
+  </si>
+  <si>
+    <t>01223456789</t>
+  </si>
+  <si>
+    <t>yusuf.bdr@gmail.com</t>
+  </si>
+  <si>
+    <t>BfhfuYwi123@</t>
+  </si>
+  <si>
+    <t>Yusuf Elsayed</t>
   </si>
 </sst>
 </file>
@@ -483,7 +525,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="25" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="23" style="1" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
     <col min="5" max="5" width="30" style="1" customWidth="1"/>
@@ -587,6 +630,66 @@
         <v>25</v>
       </c>
       <c r="F5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>